<commit_message>
refactor: Centralize styling and implement builder pattern
Centralized all styling constants into a new 'styling/style_config.py' file.
</commit_message>
<xml_diff>
--- a/result_test.xlsx
+++ b/result_test.xlsx
@@ -20,7 +20,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="33">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -132,12 +132,6 @@
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-      <color theme="1"/>
-      <sz val="10"/>
     </font>
     <font>
       <sz val="12"/>
@@ -356,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -434,122 +428,104 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1304,50 +1280,10 @@
       </c>
     </row>
     <row r="23" ht="35.1" customHeight="1"/>
-    <row r="24" ht="42" customHeight="1">
-      <c r="A24" s="31" t="inlineStr">
-        <is>
-          <t>Country of Original Cambodia</t>
-        </is>
-      </c>
-      <c r="E24" s="6" t="n"/>
-      <c r="F24" s="6" t="n"/>
-      <c r="G24" s="2" t="n"/>
-    </row>
-    <row r="25" ht="61.5" customHeight="1">
-      <c r="A25" s="32" t="inlineStr">
-        <is>
-          <t>Manufacture:</t>
-        </is>
-      </c>
-      <c r="B25" s="33" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
-XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
-        </is>
-      </c>
-      <c r="E25" s="33" t="n"/>
-      <c r="F25" s="6" t="n"/>
-      <c r="G25" s="2" t="n"/>
-    </row>
-    <row r="26" ht="42" customHeight="1">
-      <c r="A26" s="34" t="inlineStr">
-        <is>
-          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
-                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-      <c r="E26" s="34" t="n"/>
-      <c r="F26" s="34" t="n"/>
-      <c r="G26" s="2" t="n"/>
-    </row>
-    <row r="27" ht="24.75" customHeight="1">
-      <c r="A27" s="35" t="inlineStr">
-        <is>
-          <t>A/C NO:100001100764430</t>
-        </is>
-      </c>
-    </row>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
     <row r="28"/>
     <row r="29"/>
     <row r="30"/>
@@ -1522,17 +1458,13 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="7">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A27:G27"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A26:D26"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A24:D24"/>
     <mergeCell ref="B22"/>
-    <mergeCell ref="B25:D25"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1569,70 +1501,70 @@
   </cols>
   <sheetData>
     <row r="1" ht="38.25" customHeight="1">
-      <c r="A1" s="36" t="inlineStr">
+      <c r="A1" s="31" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="L1" s="37" t="n"/>
+      <c r="L1" s="32" t="n"/>
       <c r="M1" s="9" t="n"/>
     </row>
     <row r="2" ht="24" customHeight="1">
-      <c r="A2" s="38" t="inlineStr">
+      <c r="A2" s="33" t="inlineStr">
         <is>
           <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
         </is>
       </c>
-      <c r="L2" s="39" t="n"/>
+      <c r="L2" s="34" t="n"/>
       <c r="M2" s="9" t="n"/>
     </row>
     <row r="3" ht="25.5" customHeight="1">
-      <c r="A3" s="40" t="inlineStr">
+      <c r="A3" s="35" t="inlineStr">
         <is>
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
         </is>
       </c>
-      <c r="L3" s="41" t="n"/>
+      <c r="L3" s="36" t="n"/>
       <c r="M3" s="9" t="n"/>
     </row>
     <row r="4" ht="25.5" customHeight="1">
-      <c r="A4" s="38" t="inlineStr">
+      <c r="A4" s="33" t="inlineStr">
         <is>
           <t>VAT:L001-901903209</t>
         </is>
       </c>
-      <c r="L4" s="41" t="n"/>
+      <c r="L4" s="36" t="n"/>
       <c r="M4" s="9" t="n"/>
     </row>
     <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="42" t="inlineStr">
+      <c r="A5" s="37" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="L5" s="41" t="n"/>
+      <c r="L5" s="36" t="n"/>
       <c r="M5" s="9" t="n"/>
     </row>
     <row r="6" ht="54" customHeight="1">
-      <c r="A6" s="43" t="inlineStr">
+      <c r="A6" s="38" t="inlineStr">
         <is>
           <t>PACKING LIST</t>
         </is>
       </c>
-      <c r="L6" s="44" t="n"/>
+      <c r="L6" s="39" t="n"/>
       <c r="M6" s="9" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="45" t="n"/>
+      <c r="A7" s="40" t="n"/>
       <c r="B7" s="9" t="n"/>
-      <c r="C7" s="45" t="n"/>
-      <c r="D7" s="45" t="n"/>
-      <c r="E7" s="45" t="n"/>
-      <c r="F7" s="45" t="n"/>
-      <c r="G7" s="45" t="n"/>
-      <c r="H7" s="45" t="n"/>
+      <c r="C7" s="40" t="n"/>
+      <c r="D7" s="40" t="n"/>
+      <c r="E7" s="40" t="n"/>
+      <c r="F7" s="40" t="n"/>
+      <c r="G7" s="40" t="n"/>
+      <c r="H7" s="40" t="n"/>
       <c r="I7" s="9" t="n"/>
-      <c r="J7" s="46" t="inlineStr">
+      <c r="J7" s="41" t="inlineStr">
         <is>
           <t>Ref No.:</t>
         </is>
@@ -1646,21 +1578,21 @@
       <c r="M7" s="9" t="n"/>
     </row>
     <row r="8" ht="30" customHeight="1">
-      <c r="A8" s="47" t="inlineStr">
+      <c r="A8" s="42" t="inlineStr">
         <is>
           <t>EXPORTER:</t>
         </is>
       </c>
-      <c r="B8" s="48" t="inlineStr">
+      <c r="B8" s="43" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
       <c r="F8" s="9" t="n"/>
-      <c r="G8" s="49" t="n"/>
-      <c r="H8" s="49" t="n"/>
+      <c r="G8" s="44" t="n"/>
+      <c r="H8" s="44" t="n"/>
       <c r="I8" s="9" t="n"/>
-      <c r="J8" s="50" t="inlineStr">
+      <c r="J8" s="45" t="inlineStr">
         <is>
           <t>INVOICE NO :</t>
         </is>
@@ -1674,17 +1606,17 @@
       <c r="M8" s="9" t="n"/>
     </row>
     <row r="9" ht="21" customHeight="1">
-      <c r="A9" s="45" t="n"/>
-      <c r="B9" s="51" t="inlineStr">
+      <c r="A9" s="40" t="n"/>
+      <c r="B9" s="46" t="inlineStr">
         <is>
           <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages,</t>
         </is>
       </c>
       <c r="F9" s="9" t="n"/>
-      <c r="G9" s="45" t="n"/>
-      <c r="H9" s="45" t="n"/>
+      <c r="G9" s="40" t="n"/>
+      <c r="H9" s="40" t="n"/>
       <c r="I9" s="9" t="n"/>
-      <c r="J9" s="50" t="inlineStr">
+      <c r="J9" s="45" t="inlineStr">
         <is>
           <t>Date:</t>
         </is>
@@ -1698,17 +1630,17 @@
       <c r="M9" s="9" t="n"/>
     </row>
     <row r="10" ht="22.5" customHeight="1">
-      <c r="A10" s="45" t="n"/>
-      <c r="B10" s="51" t="inlineStr">
+      <c r="A10" s="40" t="n"/>
+      <c r="B10" s="46" t="inlineStr">
         <is>
           <t>Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia</t>
         </is>
       </c>
       <c r="F10" s="9" t="n"/>
-      <c r="G10" s="45" t="n"/>
-      <c r="H10" s="45" t="n"/>
+      <c r="G10" s="40" t="n"/>
+      <c r="H10" s="40" t="n"/>
       <c r="I10" s="9" t="n"/>
-      <c r="J10" s="50">
+      <c r="J10" s="45">
         <f>Invoice!F10</f>
         <v/>
       </c>
@@ -1721,17 +1653,17 @@
       <c r="M10" s="9" t="n"/>
     </row>
     <row r="11" ht="20.25" customHeight="1">
-      <c r="A11" s="45" t="n"/>
-      <c r="B11" s="51" t="inlineStr">
+      <c r="A11" s="40" t="n"/>
+      <c r="B11" s="46" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
       <c r="F11" s="9" t="n"/>
-      <c r="G11" s="45" t="n"/>
-      <c r="H11" s="45" t="n"/>
+      <c r="G11" s="40" t="n"/>
+      <c r="H11" s="40" t="n"/>
       <c r="I11" s="9" t="n"/>
-      <c r="J11" s="50" t="inlineStr">
+      <c r="J11" s="45" t="inlineStr">
         <is>
           <t>ETD：</t>
         </is>
@@ -1740,20 +1672,20 @@
         <f>K9</f>
         <v/>
       </c>
-      <c r="L11" s="39" t="n"/>
+      <c r="L11" s="34" t="n"/>
       <c r="M11" s="9" t="n"/>
     </row>
     <row r="12" ht="20.1" customHeight="1">
-      <c r="A12" s="45" t="n"/>
+      <c r="A12" s="40" t="n"/>
       <c r="B12" s="9" t="n"/>
-      <c r="C12" s="45" t="n"/>
-      <c r="D12" s="45" t="n"/>
-      <c r="E12" s="45" t="n"/>
-      <c r="F12" s="45" t="n"/>
-      <c r="G12" s="45" t="n"/>
-      <c r="H12" s="45" t="n"/>
+      <c r="C12" s="40" t="n"/>
+      <c r="D12" s="40" t="n"/>
+      <c r="E12" s="40" t="n"/>
+      <c r="F12" s="40" t="n"/>
+      <c r="G12" s="40" t="n"/>
+      <c r="H12" s="40" t="n"/>
       <c r="I12" s="9" t="n"/>
-      <c r="J12" s="50" t="inlineStr">
+      <c r="J12" s="45" t="inlineStr">
         <is>
           <t>ETA:</t>
         </is>
@@ -1762,68 +1694,68 @@
         <f>K11+1</f>
         <v/>
       </c>
-      <c r="L12" s="39" t="n"/>
+      <c r="L12" s="34" t="n"/>
       <c r="M12" s="9" t="n"/>
     </row>
     <row r="13" ht="25.5" customHeight="1">
-      <c r="A13" s="52" t="inlineStr">
+      <c r="A13" s="47" t="inlineStr">
         <is>
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="53" t="inlineStr">
+      <c r="B13" s="48" t="inlineStr">
         <is>
           <t>Wanek Furniture Co., LTD</t>
         </is>
       </c>
       <c r="F13" s="9" t="n"/>
-      <c r="G13" s="54" t="n"/>
-      <c r="H13" s="54" t="n"/>
-      <c r="I13" s="54" t="n"/>
-      <c r="J13" s="55" t="n"/>
+      <c r="G13" s="49" t="n"/>
+      <c r="H13" s="49" t="n"/>
+      <c r="I13" s="49" t="n"/>
+      <c r="J13" s="50" t="n"/>
       <c r="K13" s="9" t="n"/>
-      <c r="L13" s="39" t="n"/>
+      <c r="L13" s="34" t="n"/>
       <c r="M13" s="9" t="n"/>
     </row>
     <row r="14" ht="25.5" customHeight="1">
-      <c r="A14" s="45" t="n"/>
-      <c r="B14" s="56" t="inlineStr">
+      <c r="A14" s="40" t="n"/>
+      <c r="B14" s="51" t="inlineStr">
         <is>
           <t>Lot D_5A_CN, D_5C_CN, D_5E_CN, My Phuoc 3 Industrial Park, Thoi Hoa Ward, Ho Chi Minh City, Vietnam.</t>
         </is>
       </c>
-      <c r="F14" s="57" t="n"/>
-      <c r="G14" s="57" t="n"/>
-      <c r="H14" s="57" t="n"/>
-      <c r="I14" s="57" t="n"/>
+      <c r="F14" s="52" t="n"/>
+      <c r="G14" s="52" t="n"/>
+      <c r="H14" s="52" t="n"/>
+      <c r="I14" s="52" t="n"/>
       <c r="J14" s="9" t="n"/>
       <c r="K14" s="9" t="n"/>
-      <c r="L14" s="39" t="n"/>
+      <c r="L14" s="34" t="n"/>
       <c r="M14" s="9" t="n"/>
     </row>
     <row r="15" ht="17.25" customHeight="1">
-      <c r="A15" s="45" t="n"/>
-      <c r="B15" s="46" t="inlineStr">
+      <c r="A15" s="40" t="n"/>
+      <c r="B15" s="41" t="inlineStr">
         <is>
           <t>P+84 650 3655 200 EXT:7074 MS EMILY(C&amp;L)/MS DOROTHY(CR) EXT:7036 MS JANE (PURCHASING)</t>
         </is>
       </c>
-      <c r="F15" s="58" t="n"/>
-      <c r="G15" s="58" t="n"/>
-      <c r="H15" s="58" t="n"/>
-      <c r="I15" s="58" t="n"/>
+      <c r="F15" s="53" t="n"/>
+      <c r="G15" s="53" t="n"/>
+      <c r="H15" s="53" t="n"/>
+      <c r="I15" s="53" t="n"/>
       <c r="J15" s="9" t="n"/>
       <c r="K15" s="9" t="n"/>
-      <c r="L15" s="39" t="n"/>
+      <c r="L15" s="34" t="n"/>
       <c r="M15" s="9" t="n"/>
     </row>
     <row r="16" ht="27.75" customHeight="1">
-      <c r="A16" s="59" t="inlineStr">
+      <c r="A16" s="54" t="inlineStr">
         <is>
           <t xml:space="preserve">SHIP: </t>
         </is>
       </c>
-      <c r="B16" s="51" t="inlineStr">
+      <c r="B16" s="46" t="inlineStr">
         <is>
           <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO HO CHI MINH, VIETNAM.</t>
         </is>
@@ -1831,17 +1763,17 @@
       <c r="F16" s="9" t="n"/>
       <c r="G16" s="9" t="n"/>
       <c r="H16" s="9" t="n"/>
-      <c r="I16" s="60" t="n"/>
+      <c r="I16" s="55" t="n"/>
       <c r="J16" s="9" t="n"/>
       <c r="K16" s="9" t="n"/>
       <c r="L16" s="9" t="n"/>
       <c r="M16" s="9" t="n"/>
     </row>
     <row r="17" ht="24" customHeight="1">
-      <c r="A17" s="61" t="n"/>
+      <c r="A17" s="56" t="n"/>
       <c r="B17" s="9" t="n"/>
-      <c r="C17" s="61" t="n"/>
-      <c r="D17" s="61" t="n"/>
+      <c r="C17" s="56" t="n"/>
+      <c r="D17" s="56" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
       <c r="G17" s="9" t="n"/>
@@ -1884,7 +1816,7 @@
           <t>Quantity</t>
         </is>
       </c>
-      <c r="G18" s="62" t="n"/>
+      <c r="G18" s="57" t="n"/>
       <c r="H18" s="27" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -1907,11 +1839,11 @@
       </c>
     </row>
     <row r="19" ht="31.1" customHeight="1">
-      <c r="A19" s="63" t="n"/>
-      <c r="B19" s="63" t="n"/>
-      <c r="C19" s="63" t="n"/>
-      <c r="D19" s="63" t="n"/>
-      <c r="E19" s="63" t="n"/>
+      <c r="A19" s="58" t="n"/>
+      <c r="B19" s="58" t="n"/>
+      <c r="C19" s="58" t="n"/>
+      <c r="D19" s="58" t="n"/>
+      <c r="E19" s="58" t="n"/>
       <c r="F19" s="27" t="inlineStr">
         <is>
           <t>PCS</t>
@@ -1922,13 +1854,13 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="H19" s="63" t="n"/>
-      <c r="I19" s="63" t="n"/>
-      <c r="J19" s="63" t="n"/>
-      <c r="K19" s="63" t="n"/>
+      <c r="H19" s="58" t="n"/>
+      <c r="I19" s="58" t="n"/>
+      <c r="J19" s="58" t="n"/>
+      <c r="K19" s="58" t="n"/>
     </row>
     <row r="20" ht="31.1" customHeight="1">
-      <c r="A20" s="64" t="inlineStr">
+      <c r="A20" s="59" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
@@ -1939,7 +1871,7 @@
           <t>PT1ZX64</t>
         </is>
       </c>
-      <c r="D20" s="65" t="n">
+      <c r="D20" s="60" t="n">
         <v>140499</v>
       </c>
       <c r="E20" s="29" t="inlineStr">
@@ -1969,7 +1901,7 @@
       <c r="K20" s="29" t="n"/>
     </row>
     <row r="21" ht="31.1" customHeight="1">
-      <c r="A21" s="64" t="inlineStr">
+      <c r="A21" s="59" t="inlineStr">
         <is>
           <t>Des: L MINDANAO BUFFALO STEELU59504</t>
         </is>
@@ -1980,7 +1912,7 @@
           <t>PT1ZX64</t>
         </is>
       </c>
-      <c r="D21" s="65" t="n">
+      <c r="D21" s="60" t="n">
         <v>140499</v>
       </c>
       <c r="E21" s="29" t="inlineStr">
@@ -2010,7 +1942,7 @@
       <c r="K21" s="29" t="n"/>
     </row>
     <row r="22" ht="31.1" customHeight="1">
-      <c r="A22" s="64" t="inlineStr">
+      <c r="A22" s="59" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
@@ -2021,7 +1953,7 @@
           <t>PT1ZX64</t>
         </is>
       </c>
-      <c r="D22" s="65" t="n">
+      <c r="D22" s="60" t="n">
         <v>140499</v>
       </c>
       <c r="E22" s="29" t="inlineStr">
@@ -2051,7 +1983,7 @@
       <c r="K22" s="29" t="n"/>
     </row>
     <row r="23" ht="31.1" customHeight="1">
-      <c r="A23" s="64" t="inlineStr">
+      <c r="A23" s="59" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
@@ -2062,7 +1994,7 @@
           <t>PT1ZX64</t>
         </is>
       </c>
-      <c r="D23" s="65" t="n">
+      <c r="D23" s="60" t="n">
         <v>140499</v>
       </c>
       <c r="E23" s="29" t="inlineStr">
@@ -2092,14 +2024,14 @@
       <c r="K23" s="29" t="n"/>
     </row>
     <row r="24" ht="31.1" customHeight="1">
-      <c r="A24" s="64" t="n"/>
+      <c r="A24" s="59" t="n"/>
       <c r="B24" s="29" t="n"/>
       <c r="C24" s="29" t="inlineStr">
         <is>
           <t>PT1ZX64</t>
         </is>
       </c>
-      <c r="D24" s="65" t="n">
+      <c r="D24" s="60" t="n">
         <v>140499</v>
       </c>
       <c r="E24" s="29" t="inlineStr">
@@ -2129,14 +2061,14 @@
       <c r="K24" s="29" t="n"/>
     </row>
     <row r="25" ht="31.1" customHeight="1">
-      <c r="A25" s="64" t="n"/>
+      <c r="A25" s="59" t="n"/>
       <c r="B25" s="29" t="n"/>
       <c r="C25" s="29" t="inlineStr">
         <is>
           <t>PT1ZX64</t>
         </is>
       </c>
-      <c r="D25" s="65" t="n">
+      <c r="D25" s="60" t="n">
         <v>140499</v>
       </c>
       <c r="E25" s="29" t="inlineStr">
@@ -2170,14 +2102,14 @@
       </c>
     </row>
     <row r="26" ht="31.1" customHeight="1">
-      <c r="A26" s="64" t="n"/>
+      <c r="A26" s="59" t="n"/>
       <c r="B26" s="29" t="n"/>
       <c r="C26" s="29" t="inlineStr">
         <is>
           <t>PT1ZX64</t>
         </is>
       </c>
-      <c r="D26" s="65" t="n">
+      <c r="D26" s="60" t="n">
         <v>140499</v>
       </c>
       <c r="E26" s="29" t="inlineStr">
@@ -2207,14 +2139,14 @@
       <c r="K26" s="29" t="n"/>
     </row>
     <row r="27" ht="31.1" customHeight="1">
-      <c r="A27" s="64" t="n"/>
+      <c r="A27" s="59" t="n"/>
       <c r="B27" s="29" t="n"/>
       <c r="C27" s="29" t="inlineStr">
         <is>
           <t>PT1ZX64</t>
         </is>
       </c>
-      <c r="D27" s="65" t="n">
+      <c r="D27" s="60" t="n">
         <v>140499</v>
       </c>
       <c r="E27" s="29" t="inlineStr">
@@ -2244,14 +2176,14 @@
       <c r="K27" s="29" t="n"/>
     </row>
     <row r="28" ht="31.1" customHeight="1">
-      <c r="A28" s="64" t="n"/>
+      <c r="A28" s="59" t="n"/>
       <c r="B28" s="29" t="n"/>
       <c r="C28" s="29" t="inlineStr">
         <is>
           <t>PT1ZX64</t>
         </is>
       </c>
-      <c r="D28" s="65" t="n">
+      <c r="D28" s="60" t="n">
         <v>140499</v>
       </c>
       <c r="E28" s="29" t="inlineStr">
@@ -2281,14 +2213,14 @@
       <c r="K28" s="29" t="n"/>
     </row>
     <row r="29" ht="31.1" customHeight="1">
-      <c r="A29" s="64" t="n"/>
+      <c r="A29" s="59" t="n"/>
       <c r="B29" s="29" t="n"/>
       <c r="C29" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D29" s="65" t="n">
+      <c r="D29" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E29" s="29" t="inlineStr">
@@ -2319,14 +2251,14 @@
       <c r="K29" s="29" t="n"/>
     </row>
     <row r="30" ht="31.1" customHeight="1">
-      <c r="A30" s="64" t="n"/>
+      <c r="A30" s="59" t="n"/>
       <c r="B30" s="29" t="n"/>
       <c r="C30" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D30" s="65" t="n">
+      <c r="D30" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E30" s="29" t="inlineStr">
@@ -2357,14 +2289,14 @@
       <c r="K30" s="29" t="n"/>
     </row>
     <row r="31" ht="31.1" customHeight="1">
-      <c r="A31" s="64" t="n"/>
+      <c r="A31" s="59" t="n"/>
       <c r="B31" s="29" t="n"/>
       <c r="C31" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D31" s="65" t="n">
+      <c r="D31" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E31" s="29" t="inlineStr">
@@ -2395,14 +2327,14 @@
       <c r="K31" s="29" t="n"/>
     </row>
     <row r="32" ht="31.1" customHeight="1">
-      <c r="A32" s="64" t="n"/>
+      <c r="A32" s="59" t="n"/>
       <c r="B32" s="29" t="n"/>
       <c r="C32" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D32" s="65" t="n">
+      <c r="D32" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E32" s="29" t="inlineStr">
@@ -2433,14 +2365,14 @@
       <c r="K32" s="29" t="n"/>
     </row>
     <row r="33" ht="31.1" customHeight="1">
-      <c r="A33" s="64" t="n"/>
+      <c r="A33" s="59" t="n"/>
       <c r="B33" s="29" t="n"/>
       <c r="C33" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D33" s="65" t="n">
+      <c r="D33" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E33" s="29" t="inlineStr">
@@ -2471,14 +2403,14 @@
       <c r="K33" s="29" t="n"/>
     </row>
     <row r="34" ht="31.1" customHeight="1">
-      <c r="A34" s="64" t="n"/>
+      <c r="A34" s="59" t="n"/>
       <c r="B34" s="29" t="n"/>
       <c r="C34" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D34" s="65" t="n">
+      <c r="D34" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E34" s="29" t="inlineStr">
@@ -2509,14 +2441,14 @@
       <c r="K34" s="29" t="n"/>
     </row>
     <row r="35" ht="31.1" customHeight="1">
-      <c r="A35" s="64" t="n"/>
+      <c r="A35" s="59" t="n"/>
       <c r="B35" s="29" t="n"/>
       <c r="C35" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D35" s="65" t="n">
+      <c r="D35" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E35" s="29" t="inlineStr">
@@ -2547,14 +2479,14 @@
       <c r="K35" s="29" t="n"/>
     </row>
     <row r="36" ht="31.1" customHeight="1">
-      <c r="A36" s="64" t="n"/>
+      <c r="A36" s="59" t="n"/>
       <c r="B36" s="29" t="n"/>
       <c r="C36" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D36" s="65" t="n">
+      <c r="D36" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E36" s="29" t="inlineStr">
@@ -2585,14 +2517,14 @@
       <c r="K36" s="29" t="n"/>
     </row>
     <row r="37" ht="31.1" customHeight="1">
-      <c r="A37" s="64" t="n"/>
+      <c r="A37" s="59" t="n"/>
       <c r="B37" s="29" t="n"/>
       <c r="C37" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D37" s="65" t="n">
+      <c r="D37" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E37" s="29" t="inlineStr">
@@ -2623,14 +2555,14 @@
       <c r="K37" s="29" t="n"/>
     </row>
     <row r="38" ht="31.1" customHeight="1">
-      <c r="A38" s="64" t="n"/>
+      <c r="A38" s="59" t="n"/>
       <c r="B38" s="29" t="n"/>
       <c r="C38" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D38" s="65" t="n">
+      <c r="D38" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E38" s="29" t="inlineStr">
@@ -2665,14 +2597,14 @@
       </c>
     </row>
     <row r="39" ht="31.1" customHeight="1">
-      <c r="A39" s="64" t="n"/>
+      <c r="A39" s="59" t="n"/>
       <c r="B39" s="29" t="n"/>
       <c r="C39" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D39" s="65" t="n">
+      <c r="D39" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E39" s="29" t="inlineStr">
@@ -2703,14 +2635,14 @@
       <c r="K39" s="29" t="n"/>
     </row>
     <row r="40" ht="31.1" customHeight="1">
-      <c r="A40" s="64" t="n"/>
+      <c r="A40" s="59" t="n"/>
       <c r="B40" s="29" t="n"/>
       <c r="C40" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D40" s="65" t="n">
+      <c r="D40" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E40" s="29" t="inlineStr">
@@ -2741,14 +2673,14 @@
       <c r="K40" s="29" t="n"/>
     </row>
     <row r="41" ht="31.1" customHeight="1">
-      <c r="A41" s="64" t="n"/>
+      <c r="A41" s="59" t="n"/>
       <c r="B41" s="29" t="n"/>
       <c r="C41" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D41" s="65" t="n">
+      <c r="D41" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E41" s="29" t="inlineStr">
@@ -2779,14 +2711,14 @@
       <c r="K41" s="29" t="n"/>
     </row>
     <row r="42" ht="31.1" customHeight="1">
-      <c r="A42" s="64" t="n"/>
+      <c r="A42" s="59" t="n"/>
       <c r="B42" s="29" t="n"/>
       <c r="C42" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D42" s="65" t="n">
+      <c r="D42" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E42" s="29" t="inlineStr">
@@ -2817,14 +2749,14 @@
       <c r="K42" s="29" t="n"/>
     </row>
     <row r="43" ht="31.1" customHeight="1">
-      <c r="A43" s="64" t="n"/>
+      <c r="A43" s="59" t="n"/>
       <c r="B43" s="29" t="n"/>
       <c r="C43" s="29" t="inlineStr">
         <is>
           <t>PT26792</t>
         </is>
       </c>
-      <c r="D43" s="65" t="n">
+      <c r="D43" s="60" t="n">
         <v>140519</v>
       </c>
       <c r="E43" s="29" t="inlineStr">
@@ -2859,14 +2791,14 @@
       </c>
     </row>
     <row r="44" ht="31.1" customHeight="1">
-      <c r="A44" s="64" t="n"/>
+      <c r="A44" s="59" t="n"/>
       <c r="B44" s="29" t="n"/>
       <c r="C44" s="29" t="inlineStr">
         <is>
           <t>PT26F87</t>
         </is>
       </c>
-      <c r="D44" s="65" t="n">
+      <c r="D44" s="60" t="n">
         <v>140522</v>
       </c>
       <c r="E44" s="29" t="inlineStr">
@@ -2896,14 +2828,14 @@
       <c r="K44" s="29" t="n"/>
     </row>
     <row r="45" ht="31.1" customHeight="1">
-      <c r="A45" s="64" t="n"/>
+      <c r="A45" s="59" t="n"/>
       <c r="B45" s="29" t="n"/>
       <c r="C45" s="29" t="inlineStr">
         <is>
           <t>PT26F87</t>
         </is>
       </c>
-      <c r="D45" s="65" t="n">
+      <c r="D45" s="60" t="n">
         <v>140522</v>
       </c>
       <c r="E45" s="29" t="inlineStr">
@@ -2933,14 +2865,14 @@
       <c r="K45" s="29" t="n"/>
     </row>
     <row r="46" ht="31.1" customHeight="1">
-      <c r="A46" s="64" t="n"/>
+      <c r="A46" s="59" t="n"/>
       <c r="B46" s="29" t="n"/>
       <c r="C46" s="29" t="inlineStr">
         <is>
           <t>PT27781</t>
         </is>
       </c>
-      <c r="D46" s="65" t="n">
+      <c r="D46" s="60" t="n">
         <v>140491</v>
       </c>
       <c r="E46" s="29" t="inlineStr">
@@ -2970,7 +2902,7 @@
       <c r="K46" s="29" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="66" t="n"/>
+      <c r="A47" s="61" t="n"/>
       <c r="B47" s="29" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
@@ -3038,7 +2970,7 @@
           <t>Quantity</t>
         </is>
       </c>
-      <c r="G49" s="62" t="n"/>
+      <c r="G49" s="57" t="n"/>
       <c r="H49" s="27" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -3061,11 +2993,11 @@
       </c>
     </row>
     <row r="50" ht="31.1" customHeight="1">
-      <c r="A50" s="63" t="n"/>
-      <c r="B50" s="63" t="n"/>
-      <c r="C50" s="63" t="n"/>
-      <c r="D50" s="63" t="n"/>
-      <c r="E50" s="63" t="n"/>
+      <c r="A50" s="58" t="n"/>
+      <c r="B50" s="58" t="n"/>
+      <c r="C50" s="58" t="n"/>
+      <c r="D50" s="58" t="n"/>
+      <c r="E50" s="58" t="n"/>
       <c r="F50" s="27" t="inlineStr">
         <is>
           <t>PCS</t>
@@ -3076,13 +3008,13 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="H50" s="63" t="n"/>
-      <c r="I50" s="63" t="n"/>
-      <c r="J50" s="63" t="n"/>
-      <c r="K50" s="63" t="n"/>
+      <c r="H50" s="58" t="n"/>
+      <c r="I50" s="58" t="n"/>
+      <c r="J50" s="58" t="n"/>
+      <c r="K50" s="58" t="n"/>
     </row>
     <row r="51" ht="31.1" customHeight="1">
-      <c r="A51" s="64" t="inlineStr">
+      <c r="A51" s="59" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
@@ -3093,7 +3025,7 @@
           <t>PT27779</t>
         </is>
       </c>
-      <c r="D51" s="65" t="n">
+      <c r="D51" s="60" t="n">
         <v>140491</v>
       </c>
       <c r="E51" s="29" t="inlineStr">
@@ -3104,7 +3036,7 @@
       <c r="F51" s="29" t="n">
         <v>270</v>
       </c>
-      <c r="G51" s="65" t="n">
+      <c r="G51" s="60" t="n">
         <v>10074</v>
       </c>
       <c r="H51" s="30" t="n">
@@ -3123,7 +3055,7 @@
       <c r="K51" s="29" t="n"/>
     </row>
     <row r="52" ht="31.1" customHeight="1">
-      <c r="A52" s="64" t="inlineStr">
+      <c r="A52" s="59" t="inlineStr">
         <is>
           <t>Des: L MINDANAO BUFFALO STEELU59504</t>
         </is>
@@ -3134,7 +3066,7 @@
           <t>PT27779</t>
         </is>
       </c>
-      <c r="D52" s="65" t="n">
+      <c r="D52" s="60" t="n">
         <v>140491</v>
       </c>
       <c r="E52" s="29" t="inlineStr">
@@ -3164,7 +3096,7 @@
       <c r="K52" s="29" t="n"/>
     </row>
     <row r="53" ht="31.1" customHeight="1">
-      <c r="A53" s="64" t="inlineStr">
+      <c r="A53" s="59" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
@@ -3175,7 +3107,7 @@
           <t>PT27784</t>
         </is>
       </c>
-      <c r="D53" s="65" t="n">
+      <c r="D53" s="60" t="n">
         <v>140491</v>
       </c>
       <c r="E53" s="29" t="inlineStr">
@@ -3205,7 +3137,7 @@
       <c r="K53" s="29" t="n"/>
     </row>
     <row r="54" ht="31.1" customHeight="1">
-      <c r="A54" s="64" t="inlineStr">
+      <c r="A54" s="59" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
@@ -3216,7 +3148,7 @@
           <t>PT27784</t>
         </is>
       </c>
-      <c r="D54" s="65" t="n">
+      <c r="D54" s="60" t="n">
         <v>140491</v>
       </c>
       <c r="E54" s="29" t="inlineStr">
@@ -3246,14 +3178,14 @@
       <c r="K54" s="29" t="n"/>
     </row>
     <row r="55" ht="31.1" customHeight="1">
-      <c r="A55" s="64" t="n"/>
+      <c r="A55" s="59" t="n"/>
       <c r="B55" s="29" t="n"/>
       <c r="C55" s="29" t="inlineStr">
         <is>
           <t>PT27T94</t>
         </is>
       </c>
-      <c r="D55" s="65" t="n">
+      <c r="D55" s="60" t="n">
         <v>140478</v>
       </c>
       <c r="E55" s="29" t="inlineStr">
@@ -3283,14 +3215,14 @@
       <c r="K55" s="29" t="n"/>
     </row>
     <row r="56" ht="31.1" customHeight="1">
-      <c r="A56" s="64" t="n"/>
+      <c r="A56" s="59" t="n"/>
       <c r="B56" s="29" t="n"/>
       <c r="C56" s="29" t="inlineStr">
         <is>
           <t>PT27T94</t>
         </is>
       </c>
-      <c r="D56" s="65" t="n">
+      <c r="D56" s="60" t="n">
         <v>140478</v>
       </c>
       <c r="E56" s="29" t="inlineStr">
@@ -3320,14 +3252,14 @@
       <c r="K56" s="29" t="n"/>
     </row>
     <row r="57" ht="31.1" customHeight="1">
-      <c r="A57" s="64" t="n"/>
+      <c r="A57" s="59" t="n"/>
       <c r="B57" s="29" t="n"/>
       <c r="C57" s="29" t="inlineStr">
         <is>
           <t>PT27T94</t>
         </is>
       </c>
-      <c r="D57" s="65" t="n">
+      <c r="D57" s="60" t="n">
         <v>140478</v>
       </c>
       <c r="E57" s="29" t="inlineStr">
@@ -3357,14 +3289,14 @@
       <c r="K57" s="29" t="n"/>
     </row>
     <row r="58" ht="31.1" customHeight="1">
-      <c r="A58" s="64" t="n"/>
+      <c r="A58" s="59" t="n"/>
       <c r="B58" s="29" t="n"/>
       <c r="C58" s="29" t="inlineStr">
         <is>
           <t>PT27T94</t>
         </is>
       </c>
-      <c r="D58" s="65" t="n">
+      <c r="D58" s="60" t="n">
         <v>140478</v>
       </c>
       <c r="E58" s="29" t="inlineStr">
@@ -3375,7 +3307,7 @@
       <c r="F58" s="29" t="n">
         <v>255</v>
       </c>
-      <c r="G58" s="65" t="n">
+      <c r="G58" s="60" t="n">
         <v>10497</v>
       </c>
       <c r="H58" s="30" t="n">
@@ -3394,14 +3326,14 @@
       <c r="K58" s="29" t="n"/>
     </row>
     <row r="59" ht="31.1" customHeight="1">
-      <c r="A59" s="64" t="n"/>
+      <c r="A59" s="59" t="n"/>
       <c r="B59" s="29" t="n"/>
       <c r="C59" s="29" t="inlineStr">
         <is>
           <t>PT27T94</t>
         </is>
       </c>
-      <c r="D59" s="65" t="n">
+      <c r="D59" s="60" t="n">
         <v>140478</v>
       </c>
       <c r="E59" s="29" t="inlineStr">
@@ -3431,14 +3363,14 @@
       <c r="K59" s="29" t="n"/>
     </row>
     <row r="60" ht="31.1" customHeight="1">
-      <c r="A60" s="64" t="n"/>
+      <c r="A60" s="59" t="n"/>
       <c r="B60" s="29" t="n"/>
       <c r="C60" s="29" t="inlineStr">
         <is>
           <t>PT28714</t>
         </is>
       </c>
-      <c r="D60" s="65" t="n">
+      <c r="D60" s="60" t="n">
         <v>140467</v>
       </c>
       <c r="E60" s="29" t="inlineStr">
@@ -3468,14 +3400,14 @@
       <c r="K60" s="29" t="n"/>
     </row>
     <row r="61" ht="31.1" customHeight="1">
-      <c r="A61" s="64" t="n"/>
+      <c r="A61" s="59" t="n"/>
       <c r="B61" s="29" t="n"/>
       <c r="C61" s="29" t="inlineStr">
         <is>
           <t>PT28714</t>
         </is>
       </c>
-      <c r="D61" s="65" t="n">
+      <c r="D61" s="60" t="n">
         <v>140467</v>
       </c>
       <c r="E61" s="29" t="inlineStr">
@@ -3509,14 +3441,14 @@
       </c>
     </row>
     <row r="62" ht="31.1" customHeight="1">
-      <c r="A62" s="64" t="n"/>
+      <c r="A62" s="59" t="n"/>
       <c r="B62" s="29" t="n"/>
       <c r="C62" s="29" t="inlineStr">
         <is>
           <t>PT28714</t>
         </is>
       </c>
-      <c r="D62" s="65" t="n">
+      <c r="D62" s="60" t="n">
         <v>140467</v>
       </c>
       <c r="E62" s="29" t="inlineStr">
@@ -3546,7 +3478,7 @@
       <c r="K62" s="29" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" s="66" t="n"/>
+      <c r="A63" s="61" t="n"/>
       <c r="B63" s="29" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
@@ -3582,7 +3514,7 @@
       <c r="K63" s="29" t="n"/>
     </row>
     <row r="64" ht="31.1" customHeight="1">
-      <c r="A64" s="66" t="n"/>
+      <c r="A64" s="61" t="n"/>
       <c r="B64" s="29" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
@@ -3618,19 +3550,17 @@
       <c r="K64" s="29" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="66" t="n"/>
-      <c r="B65" s="67" t="inlineStr">
+      <c r="B65" s="29" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="C65" s="67" t="inlineStr">
+      <c r="C65" s="29" t="inlineStr">
         <is>
           <t>BUFFALO LEATHER</t>
         </is>
       </c>
-      <c r="D65" s="29" t="n"/>
-      <c r="E65" s="67" t="inlineStr">
+      <c r="E65" s="29" t="inlineStr">
         <is>
           <t>23 PALLETS</t>
         </is>
@@ -3650,22 +3580,19 @@
       <c r="J65" s="30" t="n">
         <v>52.15319999999998</v>
       </c>
-      <c r="K65" s="29" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="66" t="n"/>
-      <c r="B66" s="67" t="inlineStr">
+      <c r="B66" s="29" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="C66" s="67" t="inlineStr">
+      <c r="C66" s="29" t="inlineStr">
         <is>
           <t>COW LEATHER</t>
         </is>
       </c>
-      <c r="D66" s="29" t="n"/>
-      <c r="E66" s="67" t="inlineStr">
+      <c r="E66" s="29" t="inlineStr">
         <is>
           <t>12 PALLETS</t>
         </is>
@@ -3685,63 +3612,62 @@
       <c r="J66" s="30" t="n">
         <v>30.0564</v>
       </c>
-      <c r="K66" s="29" t="n"/>
     </row>
     <row r="67" ht="31.1" customHeight="1"/>
     <row r="68" ht="42" customHeight="1">
-      <c r="A68" s="68" t="inlineStr">
+      <c r="A68" s="62" t="inlineStr">
         <is>
           <t>Country of Original Cambodia</t>
         </is>
       </c>
-      <c r="F68" s="68" t="n"/>
-      <c r="G68" s="45" t="n"/>
-      <c r="H68" s="45" t="n"/>
-      <c r="I68" s="45" t="n"/>
-      <c r="J68" s="38" t="n"/>
+      <c r="F68" s="62" t="n"/>
+      <c r="G68" s="40" t="n"/>
+      <c r="H68" s="40" t="n"/>
+      <c r="I68" s="40" t="n"/>
+      <c r="J68" s="33" t="n"/>
       <c r="K68" s="9" t="n"/>
-      <c r="L68" s="39" t="n"/>
-      <c r="M68" s="69" t="n"/>
+      <c r="L68" s="34" t="n"/>
+      <c r="M68" s="63" t="n"/>
     </row>
     <row r="69" ht="61.5" customHeight="1">
-      <c r="A69" s="70" t="inlineStr">
+      <c r="A69" s="64" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B69" s="71" t="inlineStr">
+      <c r="B69" s="65" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="F69" s="71" t="n"/>
-      <c r="G69" s="71" t="n"/>
-      <c r="H69" s="71" t="n"/>
-      <c r="I69" s="45" t="n"/>
-      <c r="J69" s="38" t="n"/>
+      <c r="F69" s="65" t="n"/>
+      <c r="G69" s="65" t="n"/>
+      <c r="H69" s="65" t="n"/>
+      <c r="I69" s="40" t="n"/>
+      <c r="J69" s="33" t="n"/>
       <c r="K69" s="9" t="n"/>
-      <c r="L69" s="39" t="n"/>
-      <c r="M69" s="69" t="n"/>
+      <c r="L69" s="34" t="n"/>
+      <c r="M69" s="63" t="n"/>
     </row>
     <row r="70" ht="44.1" customHeight="1">
-      <c r="A70" s="72" t="inlineStr">
+      <c r="A70" s="66" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
                                           /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="F70" s="72" t="n"/>
-      <c r="G70" s="72" t="n"/>
-      <c r="H70" s="72" t="n"/>
-      <c r="I70" s="72" t="n"/>
-      <c r="J70" s="38" t="n"/>
-      <c r="K70" s="73" t="n"/>
-      <c r="L70" s="41" t="n"/>
-      <c r="M70" s="69" t="n"/>
+      <c r="F70" s="66" t="n"/>
+      <c r="G70" s="66" t="n"/>
+      <c r="H70" s="66" t="n"/>
+      <c r="I70" s="66" t="n"/>
+      <c r="J70" s="33" t="n"/>
+      <c r="K70" s="67" t="n"/>
+      <c r="L70" s="36" t="n"/>
+      <c r="M70" s="63" t="n"/>
     </row>
     <row r="71" ht="24.75" customHeight="1">
-      <c r="A71" s="73" t="inlineStr">
+      <c r="A71" s="67" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
@@ -3749,7 +3675,7 @@
       <c r="M71" s="9" t="n"/>
     </row>
     <row r="72" ht="27" customHeight="1">
-      <c r="A72" s="73" t="inlineStr">
+      <c r="A72" s="67" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
@@ -3763,14 +3689,14 @@
       <c r="D73" s="9" t="n"/>
       <c r="E73" s="9" t="n"/>
       <c r="F73" s="9" t="n"/>
-      <c r="G73" s="45" t="n"/>
-      <c r="H73" s="45" t="n"/>
-      <c r="I73" s="69" t="inlineStr">
+      <c r="G73" s="40" t="n"/>
+      <c r="H73" s="40" t="n"/>
+      <c r="I73" s="63" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="J73" s="38" t="n"/>
+      <c r="J73" s="33" t="n"/>
       <c r="K73" s="9" t="n"/>
       <c r="L73" s="9" t="n"/>
       <c r="M73" s="9" t="n"/>
@@ -3782,9 +3708,9 @@
       <c r="D74" s="9" t="n"/>
       <c r="E74" s="9" t="n"/>
       <c r="F74" s="9" t="n"/>
-      <c r="G74" s="45" t="n"/>
-      <c r="H74" s="45" t="n"/>
-      <c r="I74" s="38" t="n"/>
+      <c r="G74" s="40" t="n"/>
+      <c r="H74" s="40" t="n"/>
+      <c r="I74" s="33" t="n"/>
       <c r="J74" s="9" t="n"/>
       <c r="K74" s="9" t="n"/>
       <c r="L74" s="9" t="n"/>
@@ -3797,9 +3723,9 @@
       <c r="D75" s="9" t="n"/>
       <c r="E75" s="9" t="n"/>
       <c r="F75" s="9" t="n"/>
-      <c r="G75" s="45" t="n"/>
-      <c r="H75" s="45" t="n"/>
-      <c r="I75" s="45" t="n"/>
+      <c r="G75" s="40" t="n"/>
+      <c r="H75" s="40" t="n"/>
+      <c r="I75" s="40" t="n"/>
       <c r="J75" s="9" t="n"/>
       <c r="K75" s="9" t="n"/>
       <c r="L75" s="9" t="n"/>
@@ -3812,9 +3738,9 @@
       <c r="D76" s="9" t="n"/>
       <c r="E76" s="9" t="n"/>
       <c r="F76" s="9" t="n"/>
-      <c r="G76" s="45" t="n"/>
-      <c r="H76" s="45" t="n"/>
-      <c r="I76" s="74" t="inlineStr">
+      <c r="G76" s="40" t="n"/>
+      <c r="H76" s="40" t="n"/>
+      <c r="I76" s="68" t="inlineStr">
         <is>
           <t>ZENG XUELI</t>
         </is>
@@ -3831,11 +3757,11 @@
       <c r="D77" s="9" t="n"/>
       <c r="E77" s="9" t="n"/>
       <c r="F77" s="9" t="n"/>
-      <c r="G77" s="45" t="n"/>
-      <c r="H77" s="45" t="n"/>
+      <c r="G77" s="40" t="n"/>
+      <c r="H77" s="40" t="n"/>
       <c r="I77" s="9" t="n"/>
-      <c r="J77" s="74" t="n"/>
-      <c r="K77" s="74" t="n"/>
+      <c r="J77" s="68" t="n"/>
+      <c r="K77" s="68" t="n"/>
       <c r="L77" s="9" t="n"/>
       <c r="M77" s="9" t="n"/>
     </row>

</xml_diff>